<commit_message>
Fixed dict error in babi
</commit_message>
<xml_diff>
--- a/src/bAbi_tasks/data/Test2.xlsx
+++ b/src/bAbi_tasks/data/Test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yogesh\Projects\SaaSGPT\src\bAbi_tasks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155E3F75-A3C7-42C7-ABC0-ED80A1B7BEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04152F5C-634A-4929-B4BB-5DEAED244B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B961CE0B-E155-43D3-8BCB-215ECC2FFE6F}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Context</t>
   </si>
   <si>
-    <t>Prompts</t>
-  </si>
-  <si>
     <t>Single Supporting Fact</t>
   </si>
   <si>
@@ -70,15 +67,18 @@
     <t>Two Supporting Facts</t>
   </si>
   <si>
+    <t>playground</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
     <t>John is in the play ground.
-John picked up the football,
+John picked up the football.
 Bob went to the kitchen.</t>
   </si>
   <si>
-    <t>playground</t>
-  </si>
-  <si>
-    <t>Labels</t>
+    <t>Queries</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,10 +463,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -474,16 +474,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -491,16 +491,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>